<commit_message>
Updating the passwords of users
</commit_message>
<xml_diff>
--- a/Application Login.xlsx
+++ b/Application Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabodh.Ghosh\Katalon Studio\iRequest DewDrops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabodh.Ghosh\git\iRequestAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,13 +35,13 @@
     <t>christiano.ronaldo@mariners.com</t>
   </si>
   <si>
-    <t>iRequest@1234</t>
-  </si>
-  <si>
     <t>george.b@mariners.com</t>
   </si>
   <si>
     <t>diego.maradona@mariners.com</t>
+  </si>
+  <si>
+    <t>iRequest@12</t>
   </si>
 </sst>
 </file>
@@ -408,10 +408,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -426,23 +429,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>